<commit_message>
Updates for comantary purposes...
- Bootloader bug fixes
-- Flash file persentage fix
-- license bool added to WiFi view
- Astetics revamp
</commit_message>
<xml_diff>
--- a/Wifi bootloader prelim CPD 7.xlsx
+++ b/Wifi bootloader prelim CPD 7.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\NeilPretorius\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Neil\Dropbox (Mernok Elektronik)\Software\Booyco HMI Utility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8D46C4-675F-454D-A05B-5248243E6B0F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95FCEE77-27CC-4731-BA44-E0474394A959}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="124">
   <si>
     <t>SOF1</t>
   </si>
@@ -121,15 +121,6 @@
     <t>h</t>
   </si>
   <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
     <t>bootinfo5</t>
   </si>
   <si>
@@ -295,9 +286,6 @@
     <t>L</t>
   </si>
   <si>
-    <t>0-1</t>
-  </si>
-  <si>
     <t>[26..519]</t>
   </si>
   <si>
@@ -314,6 +302,108 @@
   </si>
   <si>
     <t>FirmwareSubRev</t>
+  </si>
+  <si>
+    <t>BootRev</t>
+  </si>
+  <si>
+    <t>BootSub</t>
+  </si>
+  <si>
+    <t>License Status</t>
+  </si>
+  <si>
+    <t>PC Name1</t>
+  </si>
+  <si>
+    <t>PC Name2</t>
+  </si>
+  <si>
+    <t>PC Name3</t>
+  </si>
+  <si>
+    <t>PC Name4</t>
+  </si>
+  <si>
+    <t>PC Name5</t>
+  </si>
+  <si>
+    <t>PC Name6</t>
+  </si>
+  <si>
+    <t>PC Name7</t>
+  </si>
+  <si>
+    <t>PC Name8</t>
+  </si>
+  <si>
+    <t>PC Name9</t>
+  </si>
+  <si>
+    <t>PC Name10</t>
+  </si>
+  <si>
+    <t>PC Name11</t>
+  </si>
+  <si>
+    <t>PC Name12</t>
+  </si>
+  <si>
+    <t>PC Name13</t>
+  </si>
+  <si>
+    <t>PC Name14</t>
+  </si>
+  <si>
+    <t>PC Name15</t>
+  </si>
+  <si>
+    <t>PC Name16</t>
+  </si>
+  <si>
+    <t>PC Name17</t>
+  </si>
+  <si>
+    <t>PC Name18</t>
+  </si>
+  <si>
+    <t>PC Name19</t>
+  </si>
+  <si>
+    <t>PC Name20</t>
+  </si>
+  <si>
+    <t>PC Name21</t>
+  </si>
+  <si>
+    <t>PC Name22</t>
+  </si>
+  <si>
+    <t>PC Name23</t>
+  </si>
+  <si>
+    <t>PC Name24</t>
+  </si>
+  <si>
+    <t>PC Name25</t>
+  </si>
+  <si>
+    <t>PC Name26</t>
+  </si>
+  <si>
+    <t>PC Name27</t>
+  </si>
+  <si>
+    <t>PC Name28</t>
+  </si>
+  <si>
+    <t>PC Name29</t>
+  </si>
+  <si>
+    <t>PC Name30</t>
+  </si>
+  <si>
+    <t>[34..519]</t>
   </si>
 </sst>
 </file>
@@ -606,7 +696,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
@@ -689,6 +779,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1011,10 +1104,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG52"/>
+  <dimension ref="A1:AO52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AL11" sqref="AL11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,19 +1122,20 @@
     <col min="10" max="10" width="12.140625" style="6" customWidth="1"/>
     <col min="11" max="11" width="11.7109375" style="6" customWidth="1"/>
     <col min="12" max="12" width="10.5703125" style="6" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" style="6" customWidth="1"/>
-    <col min="14" max="14" width="11.28515625" style="6" customWidth="1"/>
-    <col min="15" max="15" width="10.85546875" style="6" customWidth="1"/>
-    <col min="16" max="16" width="10" style="6" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="10" style="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" style="6" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="10" style="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="27" width="11" style="6" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11" style="6" customWidth="1"/>
+    <col min="19" max="26" width="11" style="6" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="11" style="6" customWidth="1"/>
     <col min="29" max="29" width="13.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="30" max="32" width="9.140625" style="6"/>
-    <col min="33" max="33" width="11.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11" style="6" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="11.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="34" max="36" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>17</v>
       </c>
@@ -1088,9 +1182,9 @@
       <c r="AF1" s="8"/>
       <c r="AG1" s="8"/>
     </row>
-    <row r="2" spans="1:33" s="11" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:41" s="11" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -1125,7 +1219,7 @@
       <c r="AF2" s="12"/>
       <c r="AG2" s="12"/>
     </row>
-    <row r="3" spans="1:33" s="1" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" s="1" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>18</v>
       </c>
@@ -1208,21 +1302,45 @@
       <c r="AB3" s="8">
         <v>25</v>
       </c>
-      <c r="AC3" s="8" t="s">
-        <v>88</v>
+      <c r="AC3" s="8">
+        <v>26</v>
       </c>
       <c r="AD3" s="8">
+        <v>27</v>
+      </c>
+      <c r="AE3" s="33">
+        <v>28</v>
+      </c>
+      <c r="AF3" s="8">
+        <v>29</v>
+      </c>
+      <c r="AG3" s="33">
+        <v>30</v>
+      </c>
+      <c r="AH3" s="8">
+        <v>31</v>
+      </c>
+      <c r="AI3" s="33">
+        <v>32</v>
+      </c>
+      <c r="AJ3" s="8">
+        <v>33</v>
+      </c>
+      <c r="AK3" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="AL3" s="8">
         <v>520</v>
       </c>
-      <c r="AE3" s="8">
+      <c r="AM3" s="8">
         <v>521</v>
       </c>
-      <c r="AF3" s="8">
-        <v>522</v>
-      </c>
-      <c r="AG3" s="8"/>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AN3" s="8">
+        <v>521</v>
+      </c>
+      <c r="AO3" s="8"/>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1242,88 +1360,112 @@
         <v>28</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>28</v>
+        <v>93</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>16</v>
+        <v>94</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>10</v>
+        <v>95</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="L4" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="M4" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="N4" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="O4" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="P4" s="19">
+        <v>96</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="Z4" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="AH4" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI4" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="AJ4" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="AK4" s="19">
         <v>0</v>
       </c>
-      <c r="Q4" s="19">
-        <v>0</v>
-      </c>
-      <c r="R4" s="19">
-        <v>0</v>
-      </c>
-      <c r="S4" s="19">
-        <v>0</v>
-      </c>
-      <c r="T4" s="19">
-        <v>0</v>
-      </c>
-      <c r="U4" s="19">
-        <v>0</v>
-      </c>
-      <c r="V4" s="19">
-        <v>0</v>
-      </c>
-      <c r="W4" s="19">
-        <v>0</v>
-      </c>
-      <c r="X4" s="19">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="19">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="19">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="19">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="AC4" s="19">
-        <v>0</v>
-      </c>
-      <c r="AD4" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE4" s="19" t="s">
+      <c r="AL4" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="AM4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="AF4" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="AG4" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AN4" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="AO4" s="18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1343,90 +1485,114 @@
         <v>28</v>
       </c>
       <c r="G5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="K5" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="L5" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="M5" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="K5" s="19" t="s">
+      <c r="N5" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="L5" s="19" t="s">
+      <c r="O5" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="M5" s="19" t="s">
+      <c r="P5" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="N5" s="19" t="s">
+      <c r="Q5" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="O5" s="19" t="s">
+      <c r="R5" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="P5" s="19" t="s">
+      <c r="S5" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="Q5" s="19" t="s">
+      <c r="T5" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="R5" s="19" t="s">
+      <c r="U5" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="S5" s="19" t="s">
+      <c r="V5" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="T5" s="19" t="s">
+      <c r="W5" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="U5" s="19" t="s">
+      <c r="X5" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="V5" s="19" t="s">
+      <c r="Y5" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="W5" s="19" t="s">
+      <c r="Z5" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="X5" s="19" t="s">
+      <c r="AA5" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="Y5" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z5" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="AA5" s="19" t="s">
-        <v>61</v>
-      </c>
       <c r="AB5" s="31" t="s">
-        <v>89</v>
-      </c>
-      <c r="AC5" s="19">
+        <v>85</v>
+      </c>
+      <c r="AC5" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD5" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="AE5" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF5" s="19">
         <v>0</v>
       </c>
-      <c r="AD5" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE5" s="19" t="s">
+      <c r="AG5" s="19">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="19">
+        <v>0</v>
+      </c>
+      <c r="AI5" s="19">
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="19">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="19">
+        <v>0</v>
+      </c>
+      <c r="AL5" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="AM5" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="AF5" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="AG5" s="18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AN5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="AO5" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -1461,7 +1627,7 @@
       <c r="AF6" s="10"/>
       <c r="AG6" s="10"/>
     </row>
-    <row r="7" spans="1:33" s="1" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" s="1" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -1541,22 +1707,20 @@
       <c r="AA7" s="8">
         <v>24</v>
       </c>
-      <c r="AB7" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="AC7" s="8">
+      <c r="AB7" s="8">
+        <v>25</v>
+      </c>
+      <c r="AC7" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD7" s="8">
         <v>520</v>
       </c>
-      <c r="AD7" s="8">
+      <c r="AE7" s="8">
         <v>521</v>
       </c>
-      <c r="AE7" s="8">
-        <v>522</v>
-      </c>
-      <c r="AF7" s="8"/>
-      <c r="AG7" s="8"/>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1577,10 +1741,10 @@
         <v>9</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>4</v>
@@ -1592,10 +1756,10 @@
         <v>11</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1625,10 +1789,10 @@
         <v>11</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <f>COUNTA(C10:J10)</f>
         <v>8</v>
@@ -1643,10 +1807,10 @@
         <v>9</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>4</v>
@@ -1658,11 +1822,11 @@
         <v>11</v>
       </c>
       <c r="K10" s="23" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1679,7 +1843,7 @@
         <v>9</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>12</v>
@@ -1706,62 +1870,62 @@
         <v>22</v>
       </c>
       <c r="O11" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="P11" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q11" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="R11" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="S11" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="T11" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="U11" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="V11" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="W11" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="X11" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y11" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z11" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA11" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB11" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC11" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD11" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE11" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="P11" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q11" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="R11" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="S11" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="T11" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="U11" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="V11" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="W11" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="X11" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y11" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="Z11" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA11" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="AB11" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC11" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD11" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE11" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF11" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="AG11" s="30"/>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1779,7 +1943,7 @@
         <v>9</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>10</v>
@@ -1800,10 +1964,10 @@
         <v>11</v>
       </c>
       <c r="M12" s="26" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1839,13 +2003,13 @@
         <v>11</v>
       </c>
       <c r="L13" s="25" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <f>COUNTA(C14:I14)</f>
         <v>7</v>
@@ -1860,7 +2024,7 @@
         <v>9</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>4</v>
@@ -1872,12 +2036,12 @@
         <v>11</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:33" s="9" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41" s="9" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
@@ -1992,24 +2156,24 @@
       <c r="AA17" s="8">
         <v>24</v>
       </c>
-      <c r="AB17" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="AC17" s="8">
+      <c r="AB17" s="8">
+        <v>25</v>
+      </c>
+      <c r="AC17" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD17" s="8">
         <v>520</v>
       </c>
-      <c r="AD17" s="8">
+      <c r="AE17" s="8">
         <v>521</v>
-      </c>
-      <c r="AE17" s="8">
-        <v>522</v>
       </c>
       <c r="AF17" s="8"/>
       <c r="AG17" s="8"/>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B18" s="2">
         <f>COUNTA(C18:I18)</f>
@@ -2022,10 +2186,10 @@
         <v>8</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>4</v>
@@ -2037,7 +2201,7 @@
         <v>11</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.25">
@@ -2055,7 +2219,7 @@
         <v>8</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>10</v>
@@ -2070,7 +2234,7 @@
         <v>11</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.25">
@@ -2087,10 +2251,10 @@
         <v>8</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>12</v>
@@ -2117,58 +2281,58 @@
         <v>22</v>
       </c>
       <c r="O20" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="P20" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q20" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="R20" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="S20" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="T20" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="U20" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="V20" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="W20" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="X20" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y20" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z20" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA20" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB20" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC20" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD20" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE20" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF20" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="P20" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q20" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="R20" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="S20" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="T20" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="U20" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="V20" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="W20" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="X20" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y20" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="Z20" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA20" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="AB20" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC20" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD20" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE20" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF20" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="AG20"/>
     </row>
@@ -2187,10 +2351,10 @@
         <v>8</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>10</v>
@@ -2211,7 +2375,7 @@
         <v>11</v>
       </c>
       <c r="M21" s="18" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.25">
@@ -2229,7 +2393,7 @@
         <v>8</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>16</v>
@@ -2250,12 +2414,12 @@
         <v>11</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B23" s="2">
         <f t="shared" si="0"/>
@@ -2268,10 +2432,10 @@
         <v>8</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>4</v>
@@ -2283,12 +2447,12 @@
         <v>11</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" s="28" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B25" s="2">
         <f>COUNTA(C25:I25)</f>
@@ -2301,10 +2465,10 @@
         <v>8</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>4</v>
@@ -2316,12 +2480,12 @@
         <v>11</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" s="28" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B26" s="2">
         <f t="shared" ref="B26" si="1">COUNTA(C26:I26)</f>
@@ -2334,7 +2498,7 @@
         <v>8</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>10</v>
@@ -2349,7 +2513,7 @@
         <v>11</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.25">
@@ -2366,10 +2530,10 @@
         <v>8</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F27" s="19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>12</v>
@@ -2396,58 +2560,58 @@
         <v>22</v>
       </c>
       <c r="O27" s="21" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="P27" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q27" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="R27" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="S27" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="T27" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="U27" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="V27" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="W27" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="X27" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y27" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z27" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA27" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB27" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC27" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD27" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE27" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF27" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="Q27" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="R27" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="S27" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="T27" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="U27" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="V27" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="W27" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="X27" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y27" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="Z27" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA27" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="AB27" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC27" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD27" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE27" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF27" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="AG27" s="30"/>
     </row>
@@ -2466,10 +2630,10 @@
         <v>8</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F28" s="19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>10</v>
@@ -2490,7 +2654,7 @@
         <v>11</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.25">
@@ -2508,7 +2672,7 @@
         <v>8</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>16</v>
@@ -2529,12 +2693,12 @@
         <v>11</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" s="28" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B30" s="2">
         <f>COUNTA(C28:I28)</f>
@@ -2547,10 +2711,10 @@
         <v>8</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>4</v>
@@ -2562,7 +2726,7 @@
         <v>11</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.25">
@@ -2577,10 +2741,10 @@
         <v>8</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>4</v>
@@ -2592,7 +2756,7 @@
         <v>11</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:33" x14ac:dyDescent="0.25">
@@ -2607,10 +2771,10 @@
         <v>8</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>4</v>
@@ -2622,12 +2786,12 @@
         <v>11</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:33" s="9" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
@@ -2742,24 +2906,21 @@
       <c r="AA36" s="8">
         <v>24</v>
       </c>
-      <c r="AB36" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="AC36" s="8">
+      <c r="AC36" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD36" s="8">
         <v>520</v>
       </c>
-      <c r="AD36" s="8">
+      <c r="AE36" s="8">
         <v>521</v>
-      </c>
-      <c r="AE36" s="8">
-        <v>522</v>
       </c>
       <c r="AF36" s="8"/>
       <c r="AG36" s="8"/>
     </row>
     <row r="37" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A37" s="27" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B37" s="2">
         <f>COUNTA(C37:I37)</f>
@@ -2772,10 +2933,10 @@
         <v>8</v>
       </c>
       <c r="E37" s="17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>4</v>
@@ -2787,7 +2948,7 @@
         <v>11</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:33" x14ac:dyDescent="0.25">
@@ -2805,7 +2966,7 @@
         <v>8</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>10</v>
@@ -2820,7 +2981,7 @@
         <v>11</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="AG38" s="29"/>
     </row>
@@ -2838,10 +2999,10 @@
         <v>8</v>
       </c>
       <c r="E39" s="17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F39" s="19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>12</v>
@@ -2868,58 +3029,58 @@
         <v>22</v>
       </c>
       <c r="O39" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="P39" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q39" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="R39" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="S39" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="T39" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="U39" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="V39" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="W39" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="X39" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y39" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z39" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA39" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB39" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC39" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD39" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE39" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF39" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="P39" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q39" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="R39" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="S39" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="T39" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="U39" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="V39" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="W39" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="X39" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y39" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="Z39" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA39" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="AB39" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC39" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD39" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE39" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF39" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="AG39" s="30"/>
     </row>
@@ -2938,10 +3099,10 @@
         <v>8</v>
       </c>
       <c r="E40" s="17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F40" s="19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>10</v>
@@ -2962,7 +3123,7 @@
         <v>11</v>
       </c>
       <c r="M40" s="18" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="AG40" s="29"/>
     </row>
@@ -2981,7 +3142,7 @@
         <v>8</v>
       </c>
       <c r="E41" s="17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>16</v>
@@ -3002,13 +3163,13 @@
         <v>11</v>
       </c>
       <c r="L41" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="AG41" s="29"/>
     </row>
     <row r="42" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A42" s="27" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B42" s="2">
         <f t="shared" si="4"/>
@@ -3021,10 +3182,10 @@
         <v>8</v>
       </c>
       <c r="E42" s="17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G42" s="3" t="s">
         <v>4</v>
@@ -3036,7 +3197,7 @@
         <v>11</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="AG42" s="29"/>
     </row>
@@ -3045,7 +3206,7 @@
     </row>
     <row r="44" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A44" s="28" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B44" s="2">
         <f>COUNTA(C44:I44)</f>
@@ -3058,10 +3219,10 @@
         <v>8</v>
       </c>
       <c r="E44" s="17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G44" s="3" t="s">
         <v>4</v>
@@ -3073,13 +3234,13 @@
         <v>11</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="AG44" s="29"/>
     </row>
     <row r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A45" s="28" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B45" s="2">
         <f t="shared" ref="B45" si="5">COUNTA(C45:I45)</f>
@@ -3092,7 +3253,7 @@
         <v>8</v>
       </c>
       <c r="E45" s="17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>10</v>
@@ -3107,7 +3268,7 @@
         <v>11</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="AG45" s="29"/>
     </row>
@@ -3125,10 +3286,10 @@
         <v>8</v>
       </c>
       <c r="E46" s="17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F46" s="19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G46" s="3" t="s">
         <v>12</v>
@@ -3155,58 +3316,58 @@
         <v>22</v>
       </c>
       <c r="O46" s="21" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="P46" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q46" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="R46" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="S46" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="T46" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="U46" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="V46" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="W46" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="X46" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y46" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z46" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA46" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="AB46" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC46" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD46" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE46" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF46" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="Q46" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="R46" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="S46" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="T46" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="U46" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="V46" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="W46" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="X46" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y46" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="Z46" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA46" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="AB46" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC46" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD46" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE46" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF46" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="AG46" s="30"/>
     </row>
@@ -3225,10 +3386,10 @@
         <v>8</v>
       </c>
       <c r="E47" s="17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F47" s="19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G47" s="3" t="s">
         <v>10</v>
@@ -3249,7 +3410,7 @@
         <v>11</v>
       </c>
       <c r="M47" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="AG47" s="29"/>
     </row>
@@ -3268,7 +3429,7 @@
         <v>8</v>
       </c>
       <c r="E48" s="17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>16</v>
@@ -3289,12 +3450,12 @@
         <v>11</v>
       </c>
       <c r="L48" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="28" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B49" s="2">
         <f>COUNTA(C47:I47)</f>
@@ -3307,10 +3468,10 @@
         <v>8</v>
       </c>
       <c r="E49" s="17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G49" s="3" t="s">
         <v>4</v>
@@ -3322,7 +3483,7 @@
         <v>11</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -3337,10 +3498,10 @@
         <v>8</v>
       </c>
       <c r="E51" s="17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>4</v>
@@ -3352,7 +3513,7 @@
         <v>11</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -3367,10 +3528,10 @@
         <v>8</v>
       </c>
       <c r="E52" s="17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G52" s="3" t="s">
         <v>4</v>
@@ -3382,7 +3543,7 @@
         <v>11</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -3410,7 +3571,7 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
@@ -3421,7 +3582,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3429,7 +3590,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>